<commit_message>
updating TMR and DR
</commit_message>
<xml_diff>
--- a/Defect Report Project 0.xlsx
+++ b/Defect Report Project 0.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EAbe\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EAbe\Documents\Project 0\Abe_Elmoubarik_Project_0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CF742350-FBCC-4D0D-9125-CC70C8FC5442}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11C9EDAC-819B-4306-BF29-C6A386A8E5BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{37F62E84-64FF-4EC7-A4D2-C59F89555504}"/>
+    <workbookView xWindow="380" yWindow="380" windowWidth="14400" windowHeight="7270" xr2:uid="{37F62E84-64FF-4EC7-A4D2-C59F89555504}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="9">
   <si>
     <t>Defect ID</t>
   </si>
@@ -50,25 +50,19 @@
     <t>Severity</t>
   </si>
   <si>
-    <t xml:space="preserve">SP </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test </t>
-  </si>
-  <si>
     <t>Status</t>
   </si>
   <si>
-    <t>Refreshing page, or directly typing in URLs to any page besides Login, causes user to be logged out (potential feature) and entire site to become unreadable (defect) until user returns to login page. If cookies are changed to keep user logged in after navigating to new URL, a new Log Out feature must be developed.</t>
-  </si>
-  <si>
-    <t>High</t>
-  </si>
-  <si>
-    <t>Medium</t>
-  </si>
-  <si>
     <t>Submitted for Review</t>
+  </si>
+  <si>
+    <t>Expected Matrix Page but actual is Matrix Dashboard</t>
+  </si>
+  <si>
+    <t>Low</t>
+  </si>
+  <si>
+    <t>Expected Defect Reporting but actual is Report a Defect</t>
   </si>
 </sst>
 </file>
@@ -420,10 +414,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D751155-0B7A-4070-958A-7E510C2A6E55}">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -432,12 +426,10 @@
     <col min="2" max="2" width="68" customWidth="1"/>
     <col min="3" max="3" width="29.6328125" customWidth="1"/>
     <col min="4" max="4" width="24.08984375" customWidth="1"/>
-    <col min="5" max="5" width="23.7265625" customWidth="1"/>
-    <col min="6" max="6" width="25.7265625" customWidth="1"/>
-    <col min="7" max="7" width="40.54296875" customWidth="1"/>
+    <col min="5" max="5" width="40.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -453,34 +445,39 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A2">
-        <v>901</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="C3" t="s">
         <v>7</v>
       </c>
-      <c r="C2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2">
-        <v>10</v>
-      </c>
-      <c r="F2">
-        <v>801</v>
-      </c>
-      <c r="G2" t="s">
-        <v>10</v>
+      <c r="D3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>